<commit_message>
Test objective function version3
</commit_message>
<xml_diff>
--- a/docs/change-log.xlsx
+++ b/docs/change-log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>version</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>nsga-iii, m-nsga-iii</t>
+  </si>
+  <si>
+    <t>0.0.8</t>
+  </si>
+  <si>
+    <t>0.0.9</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>Fix array out of bound in ModifiedEnvironmentalSelection.java</t>
+  </si>
+  <si>
+    <t>version3</t>
   </si>
 </sst>
 </file>
@@ -363,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,9 +389,10 @@
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,8 +405,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -404,7 +423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -416,6 +435,37 @@
       </c>
       <c r="D3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>